<commit_message>
- Corrigé les numéros de groupes pour passer de 030502XXXX à 040311XXXX pour les paroisses.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20638 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2030/supergroup.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2030/supergroup.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -171,13 +171,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -489,7 +486,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -512,10 +509,10 @@
       <c r="B2" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C2" s="3">
-        <v>305020100</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2">
+        <v>403110100</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -523,10 +520,10 @@
       <c r="B3" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C3" s="3">
-        <v>305020200</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3">
+        <v>403110200</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -534,10 +531,10 @@
       <c r="B4" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C4" s="3">
-        <v>305020300</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4">
+        <v>403110300</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -545,10 +542,10 @@
       <c r="B5" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C5" s="3">
-        <v>305020400</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5">
+        <v>403110400</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -556,10 +553,10 @@
       <c r="B6" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C6" s="3">
-        <v>305020500</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6">
+        <v>403110500</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -567,10 +564,10 @@
       <c r="B7" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C7" s="3">
-        <v>305020600</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7">
+        <v>403110600</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -578,10 +575,10 @@
       <c r="B8" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C8" s="3">
-        <v>305020700</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8">
+        <v>403110700</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -589,10 +586,10 @@
       <c r="B9" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C9" s="3">
-        <v>305020800</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9">
+        <v>403110800</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -600,10 +597,10 @@
       <c r="B10" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C10" s="3">
-        <v>305020900</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10">
+        <v>403110900</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -611,10 +608,10 @@
       <c r="B11" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C11" s="3">
-        <v>305021000</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11">
+        <v>403111000</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -622,10 +619,10 @@
       <c r="B12" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C12" s="3">
-        <v>305021100</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12">
+        <v>403111100</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -633,10 +630,10 @@
       <c r="B13" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C13" s="3">
-        <v>305021200</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13">
+        <v>403111200</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -644,10 +641,10 @@
       <c r="B14" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C14" s="3">
-        <v>305021300</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14">
+        <v>403111300</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -655,10 +652,10 @@
       <c r="B15" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C15" s="3">
-        <v>305021400</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15">
+        <v>403111400</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -666,10 +663,10 @@
       <c r="B16" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C16" s="3">
-        <v>305021500</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16">
+        <v>403111500</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -677,10 +674,10 @@
       <c r="B17" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C17" s="3">
-        <v>305021600</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17">
+        <v>403111600</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -688,10 +685,10 @@
       <c r="B18" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C18" s="3">
-        <v>305021700</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18">
+        <v>403111700</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -699,10 +696,10 @@
       <c r="B19" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C19" s="3">
-        <v>305021800</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19">
+        <v>403111800</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -710,10 +707,10 @@
       <c r="B20" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C20" s="3">
-        <v>305021900</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20">
+        <v>403111900</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -721,10 +718,10 @@
       <c r="B21" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C21" s="3">
-        <v>305022000</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21">
+        <v>403112000</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -732,10 +729,10 @@
       <c r="B22" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C22" s="3">
-        <v>305022100</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22">
+        <v>403112100</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -743,10 +740,10 @@
       <c r="B23" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C23" s="3">
-        <v>305022200</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23">
+        <v>403112200</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -754,10 +751,10 @@
       <c r="B24" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C24" s="3">
-        <v>305022300</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24">
+        <v>403112300</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -765,10 +762,10 @@
       <c r="B25" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C25" s="3">
-        <v>305022400</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25">
+        <v>403112400</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -776,10 +773,10 @@
       <c r="B26" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C26" s="3">
-        <v>305022500</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26">
+        <v>403112500</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -787,10 +784,10 @@
       <c r="B27" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C27" s="3">
-        <v>305022600</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27">
+        <v>403112600</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -798,10 +795,10 @@
       <c r="B28" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C28" s="3">
-        <v>305022700</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28">
+        <v>403112700</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -809,10 +806,10 @@
       <c r="B29" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C29" s="3">
-        <v>305022800</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29">
+        <v>403112800</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -820,10 +817,10 @@
       <c r="B30" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C30" s="3">
-        <v>305022900</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30">
+        <v>403112900</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -831,10 +828,10 @@
       <c r="B31" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C31" s="3">
-        <v>305023000</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31">
+        <v>403113000</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -842,10 +839,10 @@
       <c r="B32" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C32" s="3">
-        <v>305023100</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32">
+        <v>403113100</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -853,10 +850,10 @@
       <c r="B33" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C33" s="3">
-        <v>305023200</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33">
+        <v>403113200</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -864,10 +861,10 @@
       <c r="B34" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C34" s="3">
-        <v>305023300</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34">
+        <v>403113300</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -875,10 +872,10 @@
       <c r="B35" s="2">
         <v>2030000000</v>
       </c>
-      <c r="C35" s="3">
-        <v>305023400</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C35">
+        <v>403113400</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>